<commit_message>
push random puzzle and resolve puzzle
and updated
</commit_message>
<xml_diff>
--- a/Documentation/journalDeTravail.xlsx
+++ b/Documentation/journalDeTravail.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="119">
   <si>
     <t>Jour</t>
   </si>
@@ -298,6 +298,101 @@
   </si>
   <si>
     <t>intégration des nouvelles maquettes dans la documentation, mise en page plus correcte</t>
+  </si>
+  <si>
+    <t>suppression de la storie sur l'UI, intégration des tâches sur les autres stories, création d'une storie Documentation</t>
+  </si>
+  <si>
+    <t>création des cartes, facile, moyen, ajout de UI pour résolution de puzzle, adaption des sprites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recherches sur comment ajouter une fonction zoom sur un scroll view </t>
+  </si>
+  <si>
+    <t>la carte est difficle de lire en mode difficile, 
+recherches sur anciens projets + internet</t>
+  </si>
+  <si>
+    <t>intégration d'une fonction zoom sur le puzzle</t>
+  </si>
+  <si>
+    <t>permet plus de visiblité sur les différentes cartes</t>
+  </si>
+  <si>
+    <t>création du système de résolution de puzzle, partie contrôle d'entrée sortie, avec choix de niveau</t>
+  </si>
+  <si>
+    <t>avec des placeholders au niveaux de portes pour l'instant, création d'un système de global variables, avoir des variables qui se transmettent de scene à scenes</t>
+  </si>
+  <si>
+    <t>Terminé, le resultat attendu et correcte.</t>
+  </si>
+  <si>
+    <t>ajout du système de reconnaissances des portes</t>
+  </si>
+  <si>
+    <t>Terminé, a adapter les autres cartes</t>
+  </si>
+  <si>
+    <t>Adaptation des autres cartes pour le nouveau système</t>
+  </si>
+  <si>
+    <t>ajout de prefabs, pour simplifier les choses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout des autres portes logique </t>
+  </si>
+  <si>
+    <t>ajout du code pour que les autres portes loqiue
+fonctionne</t>
+  </si>
+  <si>
+    <t>Tests des implémentation des ports, vérification que les portes réagisse bien par rapport à la table de véritée</t>
+  </si>
+  <si>
+    <t>Pas terminé</t>
+  </si>
+  <si>
+    <t>plusieur portes ne fonctionne pas comme voulu</t>
+  </si>
+  <si>
+    <t>correction des portes qui ne fonctionne pas</t>
+  </si>
+  <si>
+    <t>Ajout de couleur rouge, vert pour différiencer sortie et entrée</t>
+  </si>
+  <si>
+    <t>Certaines portes ne s'affiche pas correctement</t>
+  </si>
+  <si>
+    <t>Terminé, problèmes avec les paramtères du script GateManager</t>
+  </si>
+  <si>
+    <t>Déboggage</t>
+  </si>
+  <si>
+    <t>Création du sytème de vérification du score</t>
+  </si>
+  <si>
+    <t>renvoie au menu démaré</t>
+  </si>
+  <si>
+    <t>Création du système de puzzle aléatoire</t>
+  </si>
+  <si>
+    <t>les puzzle sont beaucoup trop facile, une porte AND, seras ajouter à la fin du puzzle difficile et moyen pour complexiquer le puzzle</t>
+  </si>
+  <si>
+    <t>Ajout du listing des scripts et dossier dans la documentation</t>
+  </si>
+  <si>
+    <t>correction de bug au niveau des préfabs</t>
+  </si>
+  <si>
+    <t>certain préfab avais écrasé les données auparavant</t>
+  </si>
+  <si>
+    <t>Implémentation de la partie création des puzzles</t>
   </si>
 </sst>
 </file>
@@ -360,16 +455,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -411,25 +503,6 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -442,7 +515,26 @@
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -462,28 +554,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:I54" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:I54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:I71" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="A1:I71"/>
   <tableColumns count="9">
-    <tableColumn id="8" name="ID" dataDxfId="3"/>
-    <tableColumn id="1" name="Jour" dataDxfId="4"/>
-    <tableColumn id="2" name="Début" dataDxfId="8"/>
-    <tableColumn id="3" name="Fin" dataDxfId="2"/>
-    <tableColumn id="9" name="Durée" dataDxfId="0">
+    <tableColumn id="8" name="ID" dataDxfId="8"/>
+    <tableColumn id="1" name="Jour" dataDxfId="7"/>
+    <tableColumn id="2" name="Début" dataDxfId="6"/>
+    <tableColumn id="3" name="Fin" dataDxfId="5"/>
+    <tableColumn id="9" name="Durée" dataDxfId="4">
       <calculatedColumnFormula>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Type de tâche" dataDxfId="1"/>
-    <tableColumn id="5" name="Description de la Tâche" dataDxfId="7"/>
-    <tableColumn id="6" name="Commentaires" dataDxfId="6"/>
-    <tableColumn id="7" name="Avancement" dataDxfId="5"/>
+    <tableColumn id="4" name="Type de tâche" dataDxfId="3"/>
+    <tableColumn id="5" name="Description de la Tâche" dataDxfId="2"/>
+    <tableColumn id="6" name="Commentaires" dataDxfId="1"/>
+    <tableColumn id="7" name="Avancement" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A1:A10" totalsRowShown="0">
-  <autoFilter ref="A1:A10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A1:A11" totalsRowShown="0">
+  <autoFilter ref="A1:A11"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Type de tâches"/>
   </tableColumns>
@@ -757,15 +849,15 @@
   <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R54"/>
+  <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
@@ -777,7 +869,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>66</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -806,1458 +898,1974 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>44683</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="16">
         <v>0.3611111111111111</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="16">
         <v>0.39930555555555558</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>3.8194444444444475E-2</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="14">
         <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>44683</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="16">
         <v>0.40972222222222227</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>0.43402777777777773</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>2.4305555555555469E-2</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="A4" s="14">
         <v>3</v>
       </c>
       <c r="B4" s="5">
         <v>44683</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
         <v>0.43402777777777773</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>0.47569444444444442</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>4.1666666666666685E-2</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="A5" s="14">
         <v>4</v>
       </c>
       <c r="B5" s="5">
         <v>44683</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <v>0.5625</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="A6" s="14">
         <v>5</v>
       </c>
       <c r="B6" s="5">
         <v>44683</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>0.62847222222222221</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>2.430555555555558E-2</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7" s="14">
         <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>44683</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="16">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>0.65972222222222221</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.388888888888884E-2</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>44683</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="16">
         <v>0.65972222222222221</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>0.69444444444444453</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>3.4722222222222321E-2</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>8</v>
       </c>
       <c r="B9" s="5">
         <v>44683</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="16">
         <v>0.69444444444444453</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>0.69652777777777775</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>2.0833333333332149E-3</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="14">
         <v>9</v>
       </c>
       <c r="B10" s="5">
         <v>44683</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="16">
         <v>0.69652777777777775</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <v>0.70486111111111116</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>8.3333333333334147E-3</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="14">
         <v>10</v>
       </c>
       <c r="B11" s="5">
         <v>44684</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="16">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>0.33680555555555558</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>3.4722222222222654E-3</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="A12" s="14">
         <v>11</v>
       </c>
       <c r="B12" s="5">
         <v>44684</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="16">
         <v>0.33680555555555558</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>0.35069444444444442</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.388888888888884E-2</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="A13" s="14">
         <v>12</v>
       </c>
       <c r="B13" s="5">
         <v>44684</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="16">
         <v>0.35069444444444442</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <v>0.39930555555555558</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>4.861111111111116E-2</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+      <c r="A14" s="14">
         <v>13</v>
       </c>
       <c r="B14" s="5">
         <v>44684</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="16">
         <v>0.40972222222222227</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <v>0.41319444444444442</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>3.4722222222221544E-3</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+      <c r="A15" s="14">
         <v>14</v>
       </c>
       <c r="B15" s="5">
         <v>44684</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="16">
         <v>0.41319444444444442</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <v>0.4375</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>2.430555555555558E-2</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
+      <c r="A16" s="14">
         <v>15</v>
       </c>
       <c r="B16" s="5">
         <v>44684</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="16">
         <v>0.44097222222222227</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <v>0.46875</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>2.7777777777777735E-2</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="A17" s="14">
         <v>16</v>
       </c>
       <c r="B17" s="5">
         <v>44684</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="16">
         <v>0.46875</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="16">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.0416666666666685E-2</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
+      <c r="A18" s="14">
         <v>17</v>
       </c>
       <c r="B18" s="5">
         <v>44684</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="16">
         <v>0.47916666666666669</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="16">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>3.1249999999999944E-2</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+      <c r="A19" s="14">
         <v>18</v>
       </c>
       <c r="B19" s="5">
         <v>44684</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="16">
         <v>0.56527777777777777</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="16">
         <v>0.56805555555555554</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>2.7777777777777679E-3</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+      <c r="A20" s="14">
         <v>19</v>
       </c>
       <c r="B20" s="5">
         <v>44684</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="16">
         <v>0.56805555555555554</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <v>0.59861111111111109</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>3.0555555555555558E-2</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I20" s="8"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
+      <c r="A21" s="14">
         <v>20</v>
       </c>
       <c r="B21" s="5">
         <v>44684</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="16">
         <v>0.59861111111111109</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="16">
         <v>0.61458333333333337</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.5972222222222276E-2</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
+      <c r="A22" s="14">
         <v>21</v>
       </c>
       <c r="B22" s="5">
         <v>44684</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="16">
         <v>0.61805555555555558</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="16">
         <v>0.62847222222222221</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.041666666666663E-2</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I22" s="8"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+      <c r="A23" s="14">
         <v>22</v>
       </c>
       <c r="B23" s="5">
         <v>44684</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="16">
         <v>0.64236111111111105</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="16">
         <v>0.69791666666666663</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>5.555555555555558E-2</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="A24" s="14">
         <v>23</v>
       </c>
       <c r="B24" s="5">
         <v>44684</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="16">
         <v>0.69791666666666663</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="16">
         <v>0.70138888888888884</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>3.4722222222222099E-3</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+      <c r="A25" s="14">
         <v>24</v>
       </c>
       <c r="B25" s="5">
         <v>44686</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="16">
         <v>0.36805555555555558</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="16">
         <v>0.3888888888888889</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="8"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+      <c r="A26" s="14">
         <v>25</v>
       </c>
       <c r="B26" s="5">
         <v>44686</v>
       </c>
-      <c r="C26" s="17">
+      <c r="C26" s="16">
         <v>0.3888888888888889</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="16">
         <v>0.39097222222222222</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>2.0833333333333259E-3</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
+      <c r="A27" s="14">
         <v>26</v>
       </c>
       <c r="B27" s="5">
         <v>44686</v>
       </c>
-      <c r="C27" s="17">
+      <c r="C27" s="16">
         <v>0.39097222222222222</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="16">
         <v>0.39930555555555558</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>8.3333333333333592E-3</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="A28" s="14">
         <v>27</v>
       </c>
       <c r="B28" s="5">
         <v>44686</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="16">
         <v>0.40972222222222227</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="16">
         <v>0.47222222222222227</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>6.25E-2</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
+      <c r="A29" s="14">
         <v>28</v>
       </c>
       <c r="B29" s="5">
         <v>44686</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C29" s="16">
         <v>0.47222222222222227</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="16">
         <v>0.49305555555555558</v>
       </c>
-      <c r="E29" s="18">
+      <c r="E29" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
+      <c r="A30" s="14">
         <v>29</v>
       </c>
       <c r="B30" s="5">
         <v>44686</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="16">
         <v>0.49305555555555558</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="16">
         <v>0.50972222222222219</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.6666666666666607E-2</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
+      <c r="A31" s="14">
         <v>30</v>
       </c>
       <c r="B31" s="5">
         <v>44686</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C31" s="16">
         <v>0.63888888888888895</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="16">
         <v>0.65625</v>
       </c>
-      <c r="E31" s="18">
+      <c r="E31" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.7361111111111049E-2</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G31" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H31" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="I31" s="10"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
+      <c r="A32" s="14">
         <v>31</v>
       </c>
       <c r="B32" s="5">
         <v>44686</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C32" s="16">
         <v>0.65625</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="16">
         <v>0.66319444444444442</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>6.9444444444444198E-3</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="G32" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="I32" s="11"/>
+      <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
+      <c r="A33" s="14">
         <v>32</v>
       </c>
       <c r="B33" s="5">
         <v>44686</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="16">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="16">
         <v>0.67152777777777783</v>
       </c>
-      <c r="E33" s="18">
+      <c r="E33" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>4.8611111111112049E-3</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="G33" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H33" s="12" t="s">
+      <c r="H33" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="I33" s="14"/>
+      <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+      <c r="A34" s="14">
         <v>33</v>
       </c>
       <c r="B34" s="5">
         <v>44686</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="16">
         <v>0.67152777777777783</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="16">
         <v>0.67847222222222225</v>
       </c>
-      <c r="E34" s="18">
+      <c r="E34" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>6.9444444444444198E-3</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="G34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="H34" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I34" s="13"/>
+      <c r="I34" s="12"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
+      <c r="A35" s="14">
         <v>34</v>
       </c>
       <c r="B35" s="5">
         <v>44686</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="16">
         <v>0.67847222222222225</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="16">
         <v>0.6875</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>9.0277777777777457E-3</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="G35" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
+      <c r="A36" s="14">
         <v>35</v>
       </c>
       <c r="B36" s="5">
         <v>44686</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="16">
         <v>0.68819444444444444</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="16">
         <v>0.69374999999999998</v>
       </c>
-      <c r="E36" s="18">
+      <c r="E36" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>5.5555555555555358E-3</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G36" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H36" s="13" t="s">
+      <c r="H36" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="I36" s="13"/>
+      <c r="I36" s="12"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
+      <c r="A37" s="14">
         <v>36</v>
       </c>
       <c r="B37" s="5">
         <v>44686</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="16">
         <v>0.69374999999999998</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="16">
         <v>0.69791666666666663</v>
       </c>
-      <c r="E37" s="18">
+      <c r="E37" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>4.1666666666666519E-3</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G37" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H37" s="9" t="s">
+      <c r="H37" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I37" s="10"/>
+      <c r="I37" s="9"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
+      <c r="A38" s="14">
         <v>37</v>
       </c>
       <c r="B38" s="5">
         <v>44686</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C38" s="16">
         <v>0.69861111111111107</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="16">
         <v>0.70208333333333339</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>3.4722222222223209E-3</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="G38" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
     </row>
     <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="15">
+      <c r="A39" s="14">
         <v>38</v>
       </c>
       <c r="B39" s="5">
         <v>44687</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="16">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="16">
         <v>0.34097222222222223</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>7.6388888888889173E-3</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="G39" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H39" s="13" t="s">
+      <c r="H39" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="I39" s="13" t="s">
+      <c r="I39" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="15">
+      <c r="A40" s="14">
         <v>39</v>
       </c>
       <c r="B40" s="5">
         <v>44687</v>
       </c>
-      <c r="C40" s="17">
+      <c r="C40" s="16">
         <v>0.34097222222222223</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="16">
         <v>0.34722222222222227</v>
       </c>
-      <c r="E40" s="18">
+      <c r="E40" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>6.2500000000000333E-3</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F40" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="G40" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="13" t="s">
+      <c r="H40" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I40" s="13" t="s">
+      <c r="I40" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A41" s="15">
+      <c r="A41" s="14">
         <v>40</v>
       </c>
       <c r="B41" s="5">
         <v>44687</v>
       </c>
-      <c r="C41" s="17">
+      <c r="C41" s="16">
         <v>0.34722222222222227</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="16">
         <v>0.37916666666666665</v>
       </c>
-      <c r="E41" s="18">
+      <c r="E41" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>3.1944444444444386E-2</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G41" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H41" s="13" t="s">
+      <c r="H41" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="I41" s="13" t="s">
+      <c r="I41" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="15">
+      <c r="A42" s="14">
         <v>41</v>
       </c>
       <c r="B42" s="5">
         <v>44687</v>
       </c>
-      <c r="C42" s="17">
+      <c r="C42" s="16">
         <v>0.37916666666666665</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="16">
         <v>0.38472222222222219</v>
       </c>
-      <c r="E42" s="18">
+      <c r="E42" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>5.5555555555555358E-3</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G42" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H42" s="13" t="s">
+      <c r="H42" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I42" s="13" t="s">
+      <c r="I42" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="15">
+      <c r="A43" s="14">
         <v>42</v>
       </c>
       <c r="B43" s="5">
         <v>44687</v>
       </c>
-      <c r="C43" s="17">
+      <c r="C43" s="16">
         <v>0.38472222222222219</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="16">
         <v>0.38750000000000001</v>
       </c>
-      <c r="E43" s="18">
+      <c r="E43" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>2.7777777777778234E-3</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="F43" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G43" s="7" t="s">
+      <c r="G43" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="15">
+      <c r="A44" s="14">
         <v>43</v>
       </c>
       <c r="B44" s="5">
         <v>44687</v>
       </c>
-      <c r="C44" s="17">
+      <c r="C44" s="16">
         <v>0.38750000000000001</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="16">
         <v>0.39930555555555558</v>
       </c>
-      <c r="E44" s="18">
+      <c r="E44" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.1805555555555569E-2</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="7" t="s">
+      <c r="G44" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H44" s="13" t="s">
+      <c r="H44" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I44" s="13" t="s">
+      <c r="I44" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="15">
-        <f>A44+1</f>
+      <c r="A45" s="14">
+        <f t="shared" ref="A45:A55" si="0">A44+1</f>
         <v>44</v>
       </c>
       <c r="B45" s="5">
         <v>44687</v>
       </c>
-      <c r="C45" s="17">
+      <c r="C45" s="16">
         <v>0.40972222222222227</v>
       </c>
-      <c r="D45" s="17">
+      <c r="D45" s="16">
         <v>0.42430555555555555</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E45" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.4583333333333282E-2</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G45" s="7" t="s">
+      <c r="G45" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H45" s="13" t="s">
+      <c r="H45" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="I45" s="13" t="s">
+      <c r="I45" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="15">
-        <f>A45+1</f>
+      <c r="A46" s="14">
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="B46" s="5">
         <v>44687</v>
       </c>
-      <c r="C46" s="17">
+      <c r="C46" s="16">
         <v>0.42430555555555555</v>
       </c>
-      <c r="D46" s="17">
+      <c r="D46" s="16">
         <v>0.43402777777777773</v>
       </c>
-      <c r="E46" s="18">
+      <c r="E46" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>9.7222222222221877E-3</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="F46" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G46" s="7" t="s">
+      <c r="G46" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="H46" s="14"/>
-      <c r="I46" s="13" t="s">
+      <c r="H46" s="13"/>
+      <c r="I46" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="15">
-        <f>A46+1</f>
+      <c r="A47" s="14">
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="B47" s="5">
         <v>44687</v>
       </c>
-      <c r="C47" s="17">
+      <c r="C47" s="16">
         <v>0.43402777777777773</v>
       </c>
-      <c r="D47" s="17">
+      <c r="D47" s="16">
         <v>0.45</v>
       </c>
-      <c r="E47" s="18">
+      <c r="E47" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.5972222222222276E-2</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="G47" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H47" s="14" t="s">
+      <c r="H47" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="I47" s="13" t="s">
+      <c r="I47" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="15">
-        <f>A47+1</f>
+      <c r="A48" s="14">
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="B48" s="5">
         <v>44687</v>
       </c>
-      <c r="C48" s="17">
+      <c r="C48" s="16">
         <v>0.45</v>
       </c>
-      <c r="D48" s="17">
+      <c r="D48" s="16">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E48" s="18">
+      <c r="E48" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>8.3333333333333037E-3</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="F48" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G48" s="7" t="s">
+      <c r="G48" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H48" s="14"/>
-      <c r="I48" s="13" t="s">
+      <c r="H48" s="13"/>
+      <c r="I48" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A49" s="15">
-        <f>A48+1</f>
+      <c r="A49" s="14">
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="B49" s="5">
         <v>44687</v>
       </c>
-      <c r="C49" s="17">
+      <c r="C49" s="16">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D49" s="17">
+      <c r="D49" s="16">
         <v>0.49583333333333335</v>
       </c>
-      <c r="E49" s="18">
+      <c r="E49" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>3.7500000000000033E-2</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="F49" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="G49" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H49" s="8" t="s">
+      <c r="H49" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="I49" s="13" t="s">
+      <c r="I49" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="15">
-        <f>A49+1</f>
+      <c r="A50" s="14">
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="B50" s="5">
         <v>44687</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C50" s="16">
         <v>0.49583333333333335</v>
       </c>
-      <c r="D50" s="17">
+      <c r="D50" s="16">
         <v>0.50902777777777775</v>
       </c>
-      <c r="E50" s="18">
+      <c r="E50" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.3194444444444398E-2</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="F50" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G50" s="7" t="s">
+      <c r="G50" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H50" s="8"/>
-      <c r="I50" s="13" t="s">
+      <c r="H50" s="7"/>
+      <c r="I50" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="15">
-        <f>A50+1</f>
+      <c r="A51" s="14">
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B51" s="5">
         <v>44687</v>
       </c>
-      <c r="C51" s="6">
+      <c r="C51" s="16">
         <v>0.5625</v>
       </c>
-      <c r="D51" s="17">
+      <c r="D51" s="16">
         <v>0.59097222222222223</v>
       </c>
-      <c r="E51" s="18">
+      <c r="E51" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>2.8472222222222232E-2</v>
       </c>
-      <c r="F51" s="7" t="s">
+      <c r="F51" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G51" s="7" t="s">
+      <c r="G51" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H51" s="8"/>
-      <c r="I51" s="13" t="s">
+      <c r="H51" s="7"/>
+      <c r="I51" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="15">
-        <f>A51+1</f>
+      <c r="A52" s="14">
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="B52" s="5">
         <v>44687</v>
       </c>
-      <c r="C52" s="17">
+      <c r="C52" s="16">
         <v>0.59097222222222223</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="16">
         <v>0.6020833333333333</v>
       </c>
-      <c r="E52" s="18">
+      <c r="E52" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.1111111111111072E-2</v>
       </c>
-      <c r="F52" s="7" t="s">
+      <c r="F52" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G52" s="7" t="s">
+      <c r="G52" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H52" s="14" t="s">
+      <c r="H52" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="I52" s="13" t="s">
+      <c r="I52" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="15">
-        <f>A52+1</f>
+      <c r="A53" s="14">
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="B53" s="5">
         <v>44687</v>
       </c>
-      <c r="C53" s="17">
+      <c r="C53" s="16">
         <v>0.6020833333333333</v>
       </c>
-      <c r="D53" s="17">
+      <c r="D53" s="16">
         <v>0.61597222222222225</v>
       </c>
-      <c r="E53" s="18">
+      <c r="E53" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>1.3888888888888951E-2</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F53" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G53" s="7" t="s">
+      <c r="G53" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H53" s="14"/>
-      <c r="I53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="12" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="15">
-        <f>A53+1</f>
+      <c r="A54" s="14">
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="B54" s="5">
         <v>44687</v>
       </c>
-      <c r="C54" s="17">
+      <c r="C54" s="16">
         <v>0.61597222222222225</v>
       </c>
-      <c r="D54" s="17">
+      <c r="D54" s="16">
         <v>0.62361111111111112</v>
       </c>
-      <c r="E54" s="18">
+      <c r="E54" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
         <v>7.6388888888888618E-3</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="F54" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G54" s="7" t="s">
+      <c r="G54" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="H54" s="14"/>
-      <c r="I54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="14">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B55" s="5">
+        <v>44690</v>
+      </c>
+      <c r="C55" s="16">
+        <v>0.3347222222222222</v>
+      </c>
+      <c r="D55" s="16">
+        <v>0.34375</v>
+      </c>
+      <c r="E55" s="17">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H55" s="13"/>
+      <c r="I55" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="14">
+        <f>A55+1</f>
+        <v>55</v>
+      </c>
+      <c r="B56" s="5">
+        <v>44690</v>
+      </c>
+      <c r="C56" s="16">
+        <v>0.35069444444444442</v>
+      </c>
+      <c r="D56" s="16">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E56" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>4.861111111111116E-2</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H56" s="13"/>
+      <c r="I56" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="14">
+        <f>A56+1</f>
+        <v>56</v>
+      </c>
+      <c r="B57" s="5">
+        <v>44690</v>
+      </c>
+      <c r="C57" s="16">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D57" s="16">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="E57" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.8749999999999933E-2</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I57" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="14">
+        <f>A57+1</f>
+        <v>57</v>
+      </c>
+      <c r="B58" s="5">
+        <v>44690</v>
+      </c>
+      <c r="C58" s="16">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="D58" s="16">
+        <v>0.44513888888888892</v>
+      </c>
+      <c r="E58" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.6666666666666718E-2</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A59" s="14">
+        <f>A58+1</f>
+        <v>58</v>
+      </c>
+      <c r="B59" s="5">
+        <v>44690</v>
+      </c>
+      <c r="C59" s="16">
+        <v>0.5625</v>
+      </c>
+      <c r="D59" s="16">
+        <v>0.66527777777777775</v>
+      </c>
+      <c r="E59" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>0.10277777777777775</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="14">
+        <f>A59+1</f>
+        <v>59</v>
+      </c>
+      <c r="B60" s="5">
+        <v>44690</v>
+      </c>
+      <c r="C60" s="16">
+        <v>0.66527777777777775</v>
+      </c>
+      <c r="D60" s="16">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E60" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>3.2638888888888884E-2</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="14">
+        <f>A60+1</f>
+        <v>60</v>
+      </c>
+      <c r="B61" s="5">
+        <v>44691</v>
+      </c>
+      <c r="C61" s="16">
+        <v>0.3354166666666667</v>
+      </c>
+      <c r="D61" s="16">
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="E61" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>3.0555555555555503E-2</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="14">
+        <f>A61+1</f>
+        <v>61</v>
+      </c>
+      <c r="B62" s="5">
+        <v>44691</v>
+      </c>
+      <c r="C62" s="16">
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="D62" s="16">
+        <v>0.3756944444444445</v>
+      </c>
+      <c r="E62" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>9.7222222222222987E-3</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H62" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="14">
+        <f>A62+1</f>
+        <v>62</v>
+      </c>
+      <c r="B63" s="5">
+        <v>44691</v>
+      </c>
+      <c r="C63" s="16">
+        <v>0.3756944444444445</v>
+      </c>
+      <c r="D63" s="16">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E63" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>6.5277777777777768E-2</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H63" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="14">
+        <f>A63+1</f>
+        <v>63</v>
+      </c>
+      <c r="B64" s="5">
+        <v>44691</v>
+      </c>
+      <c r="C64" s="16">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="D64" s="16">
+        <v>0.41805555555555557</v>
+      </c>
+      <c r="E64" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.8749999999999989E-2</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H64" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="14">
+        <f>A64+1</f>
+        <v>64</v>
+      </c>
+      <c r="B65" s="5">
+        <v>44691</v>
+      </c>
+      <c r="C65" s="16">
+        <v>0.41805555555555557</v>
+      </c>
+      <c r="D65" s="16">
+        <v>0.43124999999999997</v>
+      </c>
+      <c r="E65" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.3194444444444398E-2</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="14">
+        <f>A65+1</f>
+        <v>65</v>
+      </c>
+      <c r="B66" s="5">
+        <v>44691</v>
+      </c>
+      <c r="C66" s="16">
+        <v>0.43124999999999997</v>
+      </c>
+      <c r="D66" s="16">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E66" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>9.7222222222222987E-3</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="14">
+        <f>A66+1</f>
+        <v>66</v>
+      </c>
+      <c r="B67" s="5">
+        <v>44691</v>
+      </c>
+      <c r="C67" s="16">
+        <v>0.44513888888888892</v>
+      </c>
+      <c r="D67" s="16">
+        <v>0.45555555555555555</v>
+      </c>
+      <c r="E67" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="14">
+        <f>A67+1</f>
+        <v>67</v>
+      </c>
+      <c r="B68" s="5">
+        <v>44691</v>
+      </c>
+      <c r="C68" s="16">
+        <v>0.45624999999999999</v>
+      </c>
+      <c r="D68" s="16">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E68" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>5.4166666666666641E-2</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H68" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I68" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="14">
+        <f>A68+1</f>
+        <v>68</v>
+      </c>
+      <c r="B69" s="5">
+        <v>44691</v>
+      </c>
+      <c r="C69" s="16">
+        <v>0.5625</v>
+      </c>
+      <c r="D69" s="16">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="E69" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>4.3055555555555514E-2</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="14">
+        <f>A69+1</f>
+        <v>69</v>
+      </c>
+      <c r="B70" s="5">
+        <v>44691</v>
+      </c>
+      <c r="C70" s="16">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="D70" s="16">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E70" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>2.2916666666666696E-2</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H70" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I70" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="14">
+        <f>A70+1</f>
+        <v>70</v>
+      </c>
+      <c r="B71" s="5">
+        <v>44691</v>
+      </c>
+      <c r="C71" s="16">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D71" s="16">
+        <v>0.64861111111111114</v>
+      </c>
+      <c r="E71" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.3194444444444509E-2</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2269,32 +2877,27 @@
     <hyperlink ref="H31" r:id="rId1" location="/planning/2338/story/5220" display="https://icescrum.cpnv.ch/p/EUREKA/ - /planning/2338/story/5220"/>
     <hyperlink ref="H33" r:id="rId2" display="https://docs.unity3d.com/Packages/com.unity.2d.sprite@1.0/manual/index.html"/>
     <hyperlink ref="H37" r:id="rId3" display="https://docs.microsoft.com/en-us/dotnet/csharp/fundamentals/coding-style/coding-conventions"/>
+    <hyperlink ref="H60" r:id="rId4" location="/planning/2338/sprint/2340/story/5158/tasks/task/12005" display="/planning/2338/sprint/2340/story/5158/tasks/task/12005"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="58" orientation="landscape" r:id="rId4"/>
+  <pageSetup paperSize="8" scale="45" orientation="landscape" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Types de Tâche'!$A$2:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>L7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Types de Tâche'!$A$2:$A$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>F19:F54</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Types de Tâche'!$A$2:$A$10</xm:f>
+            <xm:f>'Types de Tâche'!$A$2:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F18</xm:sqref>
+          <xm:sqref>F2:F71</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2305,9 +2908,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2364,6 +2969,11 @@
         <v>33</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
finished "théories des portes"
and documentation push
</commit_message>
<xml_diff>
--- a/Documentation/journalDeTravail.xlsx
+++ b/Documentation/journalDeTravail.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="147">
   <si>
     <t>Jour</t>
   </si>
@@ -392,7 +392,92 @@
     <t>certain préfab avais écrasé les données auparavant</t>
   </si>
   <si>
-    <t>Implémentation de la partie création des puzzles</t>
+    <t>Implémentation de la partie création des puzzles, adaptation de l'UI, changement des portes quand le joueur choisit une porte</t>
+  </si>
+  <si>
+    <t>les cartes ont du être recréer pour s'adapter au système</t>
+  </si>
+  <si>
+    <t>push sur github, envoie du mail aux experts et chef de projet, contrôle de la documentations</t>
+  </si>
+  <si>
+    <t>Adaptation de l'ui de la création de puzzle pour les téléphones</t>
+  </si>
+  <si>
+    <t>création du script qui contrôle toutes les portes logiques et passe en mode résolution</t>
+  </si>
+  <si>
+    <t>Pas terminé, sauvegarde de la selection actuelle, il manque juste de charger la sélection sur la scène ou le puzzle sera résolu</t>
+  </si>
+  <si>
+    <t>ajout du chargemet de la sélection sur la scène de résolution de puzzle, beaucoup de problèmes lié avec ce que le joueur choissait comme puzzle et ce que la résolution affichais</t>
+  </si>
+  <si>
+    <t>création du sytème de théorie</t>
+  </si>
+  <si>
+    <t>affiche plusieur boutons avec les portes logiques</t>
+  </si>
+  <si>
+    <t>Pas terminé, manque l'affichage des portes détaillée,OR,  AND, NAND, XOR, XNOR</t>
+  </si>
+  <si>
+    <t>Ajout du reste des théories détaillé des portes logique</t>
+  </si>
+  <si>
+    <t>Ajout des tests d'acceptation sur icescrum</t>
+  </si>
+  <si>
+    <t>ajout des tests pour toutes les fonctionnalitées</t>
+  </si>
+  <si>
+    <t>Ajout des version de windows et unity, plus ajout des descriptions des nouveaux script : GeneratePuzzle, customGateManager, customPuzzle</t>
+  </si>
+  <si>
+    <t>ajout du bouton pour quitter le jeu, ajout d'icones pour le jeu</t>
+  </si>
+  <si>
+    <t>Commentage du code</t>
+  </si>
+  <si>
+    <t>certain bout de codes ne sont pas bien ou pas commenté</t>
+  </si>
+  <si>
+    <t>Ajout des tests d'acceptation éffectué dans le code</t>
+  </si>
+  <si>
+    <t>ajout des splash screen et écran d'acceuil</t>
+  </si>
+  <si>
+    <t>ajout des variables, fonctions, events des scripts dans la documentation</t>
+  </si>
+  <si>
+    <t>à changer : créer la planification détaillée, 
+ajout de stories par rapport à la documentation</t>
+  </si>
+  <si>
+    <t>Création de la planification détaillée</t>
+  </si>
+  <si>
+    <t>pas terminé, création de la semaine 1</t>
+  </si>
+  <si>
+    <t>Aide à Valentin Zingg</t>
+  </si>
+  <si>
+    <t>problèmes lié au turn right et turn left, le tank se bloque sur 0</t>
+  </si>
+  <si>
+    <t>Terminé, utilisation de la fonction Vector3.SignedAngle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajout de la planification détaillée dans </t>
+  </si>
+  <si>
+    <t>ajout des stories de documentation sur chaque sprint sur icescrum</t>
+  </si>
+  <si>
+    <t>Tests globale des fonctionnalitée en mode build</t>
   </si>
 </sst>
 </file>
@@ -501,7 +586,54 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -554,20 +686,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:I71" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:I71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:I93" totalsRowCount="1" dataDxfId="18">
+  <autoFilter ref="A1:I93"/>
   <tableColumns count="9">
-    <tableColumn id="8" name="ID" dataDxfId="8"/>
-    <tableColumn id="1" name="Jour" dataDxfId="7"/>
-    <tableColumn id="2" name="Début" dataDxfId="6"/>
-    <tableColumn id="3" name="Fin" dataDxfId="5"/>
-    <tableColumn id="9" name="Durée" dataDxfId="4">
+    <tableColumn id="8" name="ID" dataDxfId="17" totalsRowDxfId="8"/>
+    <tableColumn id="1" name="Jour" dataDxfId="16" totalsRowDxfId="7"/>
+    <tableColumn id="2" name="Début" dataDxfId="15" totalsRowDxfId="6"/>
+    <tableColumn id="3" name="Fin" dataDxfId="14" totalsRowDxfId="5"/>
+    <tableColumn id="9" name="Durée" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="0">
       <calculatedColumnFormula>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</calculatedColumnFormula>
+      <totalsRowFormula>SUM(E2:E92)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="Type de tâche" dataDxfId="3"/>
-    <tableColumn id="5" name="Description de la Tâche" dataDxfId="2"/>
-    <tableColumn id="6" name="Commentaires" dataDxfId="1"/>
-    <tableColumn id="7" name="Avancement" dataDxfId="0"/>
+    <tableColumn id="4" name="Type de tâche" dataDxfId="12" totalsRowDxfId="4"/>
+    <tableColumn id="5" name="Description de la Tâche" dataDxfId="11" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="Commentaires" dataDxfId="10" totalsRowDxfId="2"/>
+    <tableColumn id="7" name="Avancement" dataDxfId="9" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -849,22 +982,22 @@
   <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R71"/>
+  <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="140" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="56.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2385,7 +2518,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="14">
-        <f>A55+1</f>
+        <f t="shared" ref="A56:A71" si="1">A55+1</f>
         <v>55</v>
       </c>
       <c r="B56" s="5">
@@ -2414,7 +2547,7 @@
     </row>
     <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="14">
-        <f>A56+1</f>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B57" s="5">
@@ -2445,7 +2578,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="14">
-        <f>A57+1</f>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="B58" s="5">
@@ -2476,7 +2609,7 @@
     </row>
     <row r="59" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="14">
-        <f>A58+1</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="B59" s="5">
@@ -2507,7 +2640,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="14">
-        <f>A59+1</f>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="B60" s="5">
@@ -2538,7 +2671,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="14">
-        <f>A60+1</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="B61" s="5">
@@ -2569,7 +2702,7 @@
     </row>
     <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="14">
-        <f>A61+1</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="B62" s="5">
@@ -2600,7 +2733,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="14">
-        <f>A62+1</f>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="B63" s="5">
@@ -2631,7 +2764,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="14">
-        <f>A63+1</f>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="B64" s="5">
@@ -2662,7 +2795,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="14">
-        <f>A64+1</f>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="B65" s="5">
@@ -2691,7 +2824,7 @@
     </row>
     <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="14">
-        <f>A65+1</f>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="B66" s="5">
@@ -2720,7 +2853,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="14">
-        <f>A66+1</f>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="B67" s="5">
@@ -2751,7 +2884,7 @@
     </row>
     <row r="68" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="14">
-        <f>A67+1</f>
+        <f t="shared" si="1"/>
         <v>67</v>
       </c>
       <c r="B68" s="5">
@@ -2782,7 +2915,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="14">
-        <f>A68+1</f>
+        <f t="shared" si="1"/>
         <v>68</v>
       </c>
       <c r="B69" s="5">
@@ -2811,7 +2944,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="14">
-        <f>A69+1</f>
+        <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="B70" s="5">
@@ -2840,9 +2973,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="14">
-        <f>A70+1</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="B71" s="5">
@@ -2852,11 +2985,11 @@
         <v>0.63541666666666663</v>
       </c>
       <c r="D71" s="16">
-        <v>0.64861111111111114</v>
+        <v>0.69305555555555554</v>
       </c>
       <c r="E71" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
-        <v>1.3194444444444509E-2</v>
+        <v>5.7638888888888906E-2</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>9</v>
@@ -2864,8 +2997,651 @@
       <c r="G71" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
+      <c r="H71" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="I71" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="14">
+        <f>A71+1</f>
+        <v>71</v>
+      </c>
+      <c r="B72" s="5">
+        <v>44691</v>
+      </c>
+      <c r="C72" s="16">
+        <v>0.6958333333333333</v>
+      </c>
+      <c r="D72" s="16">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="E72" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>5.5555555555555358E-3</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="14">
+        <f>A72+1</f>
+        <v>72</v>
+      </c>
+      <c r="B73" s="5">
+        <v>44693</v>
+      </c>
+      <c r="C73" s="16">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D73" s="16">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="E73" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
+    </row>
+    <row r="74" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A74" s="14">
+        <f>A73+1</f>
+        <v>73</v>
+      </c>
+      <c r="B74" s="5">
+        <v>44693</v>
+      </c>
+      <c r="C74" s="16">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="D74" s="16">
+        <v>0.40069444444444446</v>
+      </c>
+      <c r="E74" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.8750000000000044E-2</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="14">
+        <f>A74+1</f>
+        <v>74</v>
+      </c>
+      <c r="B75" s="5">
+        <v>44693</v>
+      </c>
+      <c r="C75" s="16">
+        <v>0.41041666666666665</v>
+      </c>
+      <c r="D75" s="16">
+        <v>0.50972222222222219</v>
+      </c>
+      <c r="E75" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>9.9305555555555536E-2</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H75" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="I75" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="14">
+        <f>A75+1</f>
+        <v>75</v>
+      </c>
+      <c r="B76" s="5">
+        <v>44693</v>
+      </c>
+      <c r="C76" s="16">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D76" s="16">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="E76" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H76" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I76" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="14">
+        <f>A76+1</f>
+        <v>76</v>
+      </c>
+      <c r="B77" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C77" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D77" s="16">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="E77" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H77" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I77" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="14">
+        <f>A77+1</f>
+        <v>77</v>
+      </c>
+      <c r="B78" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C78" s="16">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="D78" s="16">
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="E78" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H78" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="I78" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="14">
+        <f>A78+1</f>
+        <v>78</v>
+      </c>
+      <c r="B79" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C79" s="16">
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="D79" s="16">
+        <v>0.375</v>
+      </c>
+      <c r="E79" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.6666666666666663E-2</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="14">
+        <f>A79+1</f>
+        <v>79</v>
+      </c>
+      <c r="B80" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C80" s="16">
+        <v>0.375</v>
+      </c>
+      <c r="D80" s="16">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="E80" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.2500000000000011E-2</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H80" s="12"/>
+      <c r="I80" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="14">
+        <f>A80+1</f>
+        <v>80</v>
+      </c>
+      <c r="B81" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C81" s="16">
+        <v>0.38819444444444445</v>
+      </c>
+      <c r="D81" s="16">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E81" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.1111111111111127E-2</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H81" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="I81" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="14">
+        <f>A81+1</f>
+        <v>81</v>
+      </c>
+      <c r="B82" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C82" s="16">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D82" s="16">
+        <v>0.41736111111111113</v>
+      </c>
+      <c r="E82" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>7.6388888888888618E-3</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H82" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="I82" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="14">
+        <f>A82+1</f>
+        <v>82</v>
+      </c>
+      <c r="B83" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C83" s="16">
+        <v>0.41736111111111113</v>
+      </c>
+      <c r="D83" s="16">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="E83" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.3194444444444453E-2</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H83" s="12"/>
+      <c r="I83" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="14">
+        <f>A83+1</f>
+        <v>83</v>
+      </c>
+      <c r="B84" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C84" s="16">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D84" s="16">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E84" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="14">
+        <f t="shared" ref="A85:A92" si="2">A84+1</f>
+        <v>84</v>
+      </c>
+      <c r="B85" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C85" s="16">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D85" s="16">
+        <v>0.46388888888888885</v>
+      </c>
+      <c r="E85" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.5972222222222165E-2</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H85" s="6"/>
+      <c r="I85" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="14">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="B86" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C86" s="16">
+        <v>0.46388888888888885</v>
+      </c>
+      <c r="D86" s="16">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E86" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.5277777777777835E-2</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H86" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I86" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="14">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="B87" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C87" s="16">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D87" s="16">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="E87" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H87" s="6"/>
+      <c r="I87" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="14">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="B88" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C88" s="16">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="D88" s="16">
+        <v>0.50972222222222219</v>
+      </c>
+      <c r="E88" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.3194444444444453E-2</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I88" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="14">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="B89" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C89" s="16">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="D89" s="16">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="E89" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>3.9583333333333304E-2</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I89" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="14">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+      <c r="B90" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C90" s="16">
+        <v>0.60555555555555551</v>
+      </c>
+      <c r="D90" s="16">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="E90" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>1.1111111111111183E-2</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G90" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H90" s="6"/>
+      <c r="I90" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="14">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="B91" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C91" s="16">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="D91" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="E91" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>8.3333333333333037E-3</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G91" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H91" s="6"/>
+      <c r="I91" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="14">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="B92" s="5">
+        <v>44694</v>
+      </c>
+      <c r="C92" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="D92" s="16">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E92" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G92" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H92" s="6"/>
+      <c r="I92" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="14"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="16"/>
+      <c r="E93" s="17">
+        <f>SUM(E2:E92)</f>
+        <v>2.2583333333333324</v>
+      </c>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2880,7 +3656,7 @@
     <hyperlink ref="H60" r:id="rId4" location="/planning/2338/sprint/2340/story/5158/tasks/task/12005" display="/planning/2338/sprint/2340/story/5158/tasks/task/12005"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="45" orientation="landscape" r:id="rId5"/>
+  <pageSetup paperSize="8" scale="34" orientation="landscape" r:id="rId5"/>
   <tableParts count="1">
     <tablePart r:id="rId6"/>
   </tableParts>
@@ -2897,7 +3673,7 @@
           <x14:formula1>
             <xm:f>'Types de Tâche'!$A$2:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F71</xm:sqref>
+          <xm:sqref>F2:F92</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
ajout d'un test unitaire, mise à jour de la documentation
</commit_message>
<xml_diff>
--- a/Documentation/journalDeTravail.xlsx
+++ b/Documentation/journalDeTravail.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="192">
   <si>
     <t>Jour</t>
   </si>
@@ -596,6 +596,27 @@
   </si>
   <si>
     <t>Pas terminé, encore 4 semaines à fiaire, très fastidieux</t>
+  </si>
+  <si>
+    <t>Finilasitation de la documentation, ajout du temps passé courant</t>
+  </si>
+  <si>
+    <t>Finilasitation de la documentation, ajout du temps passé courant, commentage</t>
+  </si>
+  <si>
+    <t>création de tests unitaire sur unity</t>
+  </si>
+  <si>
+    <t>gros soucis lié avec des problèmes, les tests qui fonctionnais la semaine passées ne fonctionne plus aujourd'hui, beaucoup de recherches à faire</t>
+  </si>
+  <si>
+    <t>ajout du test unitaire dans la documentation, ajout des informations du candidat, experts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problème de préfabs, hiérarchie perdue </t>
+  </si>
+  <si>
+    <t>Terminé, lors de l'ouverture du projet, il se peux que les préfabs soit cassé</t>
   </si>
 </sst>
 </file>
@@ -606,7 +627,7 @@
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,6 +657,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -658,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -697,6 +725,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -804,8 +835,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:I129" totalsRowCount="1" dataDxfId="18">
-  <autoFilter ref="A1:I128"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="A1:I136" totalsRowCount="1" dataDxfId="18">
+  <autoFilter ref="A1:I135">
+    <filterColumn colId="1">
+      <filters>
+        <dateGroupItem year="2022" month="5" day="23" dateTimeGrouping="day"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="9">
     <tableColumn id="8" name="ID" dataDxfId="17" totalsRowDxfId="8"/>
     <tableColumn id="1" name="Jour" dataDxfId="16" totalsRowDxfId="7"/>
@@ -813,7 +850,7 @@
     <tableColumn id="3" name="Fin" dataDxfId="14" totalsRowDxfId="5"/>
     <tableColumn id="9" name="Durée" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="4">
       <calculatedColumnFormula>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</calculatedColumnFormula>
-      <totalsRowFormula>SUM(E2:E128)</totalsRowFormula>
+      <totalsRowFormula>SUM(E2:E135)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" name="Type de tâche" dataDxfId="12" totalsRowDxfId="3"/>
     <tableColumn id="5" name="Description de la Tâche" dataDxfId="11" totalsRowDxfId="2"/>
@@ -1100,10 +1137,10 @@
   <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R129"/>
+  <dimension ref="A1:R136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F111" workbookViewId="0">
-      <selection activeCell="I135" sqref="I134:I135"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I135" sqref="I135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,7 +1185,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -1174,7 +1211,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -1200,7 +1237,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -1226,7 +1263,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -1252,7 +1289,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -1278,7 +1315,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -1306,7 +1343,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -1332,7 +1369,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -1358,7 +1395,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -1384,7 +1421,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -1410,7 +1447,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -1436,7 +1473,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -1462,7 +1499,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -1488,7 +1525,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>14</v>
       </c>
@@ -1514,7 +1551,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>15</v>
       </c>
@@ -1540,7 +1577,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>16</v>
       </c>
@@ -1568,7 +1605,7 @@
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -1594,7 +1631,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>18</v>
       </c>
@@ -1620,7 +1657,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>19</v>
       </c>
@@ -1648,7 +1685,7 @@
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -1674,7 +1711,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -1702,7 +1739,7 @@
       </c>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
         <v>22</v>
       </c>
@@ -1728,7 +1765,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>23</v>
       </c>
@@ -1754,7 +1791,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>24</v>
       </c>
@@ -1782,7 +1819,7 @@
       </c>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <v>25</v>
       </c>
@@ -1808,7 +1845,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
         <v>26</v>
       </c>
@@ -1834,7 +1871,7 @@
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>27</v>
       </c>
@@ -1860,7 +1897,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>28</v>
       </c>
@@ -1886,7 +1923,7 @@
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>29</v>
       </c>
@@ -1912,7 +1949,7 @@
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>30</v>
       </c>
@@ -1940,7 +1977,7 @@
       </c>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>31</v>
       </c>
@@ -1968,7 +2005,7 @@
       </c>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>32</v>
       </c>
@@ -1996,7 +2033,7 @@
       </c>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>33</v>
       </c>
@@ -2024,7 +2061,7 @@
       </c>
       <c r="I34" s="12"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
         <v>34</v>
       </c>
@@ -2050,7 +2087,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>35</v>
       </c>
@@ -2078,7 +2115,7 @@
       </c>
       <c r="I36" s="12"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
         <v>36</v>
       </c>
@@ -2106,7 +2143,7 @@
       </c>
       <c r="I37" s="9"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>37</v>
       </c>
@@ -2132,7 +2169,7 @@
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
     </row>
-    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
         <v>38</v>
       </c>
@@ -2162,7 +2199,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
         <v>39</v>
       </c>
@@ -2192,7 +2229,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
         <v>40</v>
       </c>
@@ -2222,7 +2259,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
         <v>41</v>
       </c>
@@ -2252,7 +2289,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="14">
         <v>42</v>
       </c>
@@ -2278,7 +2315,7 @@
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
     </row>
-    <row r="44" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14">
         <v>43</v>
       </c>
@@ -2308,7 +2345,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
         <f t="shared" ref="A45:A55" si="0">A44+1</f>
         <v>44</v>
@@ -2339,7 +2376,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2368,7 +2405,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2399,7 +2436,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2428,7 +2465,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2459,7 +2496,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2488,7 +2525,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2517,7 +2554,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -2548,7 +2585,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -2577,7 +2614,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -2606,7 +2643,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -2634,7 +2671,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14">
         <f t="shared" ref="A56:A71" si="1">A55+1</f>
         <v>55</v>
@@ -2663,7 +2700,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -2694,7 +2731,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -2725,7 +2762,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -2756,7 +2793,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -2787,7 +2824,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -2818,7 +2855,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -2849,7 +2886,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -2861,11 +2898,11 @@
         <v>0.3756944444444445</v>
       </c>
       <c r="D63" s="16">
-        <v>0.44097222222222227</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="E63" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
-        <v>6.5277777777777768E-2</v>
+        <v>2.3611111111111083E-2</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>8</v>
@@ -2880,7 +2917,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -2889,14 +2926,14 @@
         <v>44691</v>
       </c>
       <c r="C64" s="16">
-        <v>0.39930555555555558</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="D64" s="16">
         <v>0.41805555555555557</v>
       </c>
       <c r="E64" s="17">
         <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
-        <v>1.8749999999999989E-2</v>
+        <v>8.3333333333333037E-3</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>8</v>
@@ -2911,7 +2948,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -2940,7 +2977,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -2969,7 +3006,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -3000,7 +3037,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -3031,7 +3068,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -3060,7 +3097,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="14">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -3091,7 +3128,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="14">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -3122,7 +3159,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="14">
         <f t="shared" ref="A72:A84" si="2">A71+1</f>
         <v>71</v>
@@ -3151,7 +3188,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="14">
         <f t="shared" si="2"/>
         <v>72</v>
@@ -3178,7 +3215,7 @@
       <c r="H73" s="12"/>
       <c r="I73" s="12"/>
     </row>
-    <row r="74" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="14">
         <f t="shared" si="2"/>
         <v>73</v>
@@ -3207,7 +3244,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="14">
         <f t="shared" si="2"/>
         <v>74</v>
@@ -3238,7 +3275,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="14">
         <f t="shared" si="2"/>
         <v>75</v>
@@ -3269,7 +3306,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="14">
         <f t="shared" si="2"/>
         <v>76</v>
@@ -3300,7 +3337,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="14">
         <f t="shared" si="2"/>
         <v>77</v>
@@ -3331,7 +3368,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="14">
         <f t="shared" si="2"/>
         <v>78</v>
@@ -3360,7 +3397,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="14">
         <f t="shared" si="2"/>
         <v>79</v>
@@ -3389,7 +3426,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="14">
         <f t="shared" si="2"/>
         <v>80</v>
@@ -3420,7 +3457,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="14">
         <f t="shared" si="2"/>
         <v>81</v>
@@ -3451,7 +3488,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="14">
         <f t="shared" si="2"/>
         <v>82</v>
@@ -3480,7 +3517,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="14">
         <f t="shared" si="2"/>
         <v>83</v>
@@ -3509,9 +3546,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="14">
-        <f t="shared" ref="A85:B128" si="3">A84+1</f>
+        <f t="shared" ref="A85:A135" si="3">A84+1</f>
         <v>84</v>
       </c>
       <c r="B85" s="5">
@@ -3538,7 +3575,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14">
         <f t="shared" si="3"/>
         <v>85</v>
@@ -3569,7 +3606,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14">
         <f t="shared" si="3"/>
         <v>86</v>
@@ -3598,7 +3635,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14">
         <f t="shared" si="3"/>
         <v>87</v>
@@ -3629,7 +3666,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14">
         <f t="shared" si="3"/>
         <v>88</v>
@@ -3660,7 +3697,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14">
         <f t="shared" si="3"/>
         <v>89</v>
@@ -3689,7 +3726,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="14">
         <f t="shared" si="3"/>
         <v>90</v>
@@ -3718,7 +3755,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14">
         <f t="shared" si="3"/>
         <v>91</v>
@@ -3747,7 +3784,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="14">
         <f t="shared" si="3"/>
         <v>92</v>
@@ -3776,7 +3813,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="14">
         <f>A93+1</f>
         <v>93</v>
@@ -3807,7 +3844,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="14">
         <f t="shared" si="3"/>
         <v>94</v>
@@ -3836,7 +3873,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="14">
         <f t="shared" si="3"/>
         <v>95</v>
@@ -3865,7 +3902,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="14">
         <f t="shared" si="3"/>
         <v>96</v>
@@ -3894,7 +3931,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="14">
         <f t="shared" si="3"/>
         <v>97</v>
@@ -3923,7 +3960,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="14">
         <f t="shared" si="3"/>
         <v>98</v>
@@ -3952,7 +3989,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="14">
         <f t="shared" si="3"/>
         <v>99</v>
@@ -3983,7 +4020,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="14">
         <f t="shared" si="3"/>
         <v>100</v>
@@ -4012,7 +4049,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="14">
         <f t="shared" si="3"/>
         <v>101</v>
@@ -4041,7 +4078,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="14">
         <f t="shared" si="3"/>
         <v>102</v>
@@ -4072,7 +4109,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="14">
         <f t="shared" si="3"/>
         <v>103</v>
@@ -4101,7 +4138,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14">
         <f t="shared" si="3"/>
         <v>104</v>
@@ -4130,7 +4167,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="14">
         <f t="shared" si="3"/>
         <v>105</v>
@@ -4159,7 +4196,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="14">
         <f t="shared" si="3"/>
         <v>106</v>
@@ -4188,7 +4225,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="14">
         <f t="shared" si="3"/>
         <v>107</v>
@@ -4217,7 +4254,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="14">
         <f t="shared" si="3"/>
         <v>108</v>
@@ -4248,7 +4285,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="14">
         <f t="shared" si="3"/>
         <v>109</v>
@@ -4277,7 +4314,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="14">
         <f t="shared" si="3"/>
         <v>110</v>
@@ -4306,7 +4343,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="14">
         <f t="shared" si="3"/>
         <v>111</v>
@@ -4335,7 +4372,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="14">
         <f t="shared" si="3"/>
         <v>112</v>
@@ -4364,7 +4401,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="14">
         <f t="shared" si="3"/>
         <v>113</v>
@@ -4395,7 +4432,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="14">
         <f t="shared" si="3"/>
         <v>114</v>
@@ -4424,7 +4461,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="14">
         <f t="shared" si="3"/>
         <v>115</v>
@@ -4455,7 +4492,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="14">
         <f t="shared" si="3"/>
         <v>116</v>
@@ -4486,7 +4523,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="14">
         <f t="shared" si="3"/>
         <v>117</v>
@@ -4517,7 +4554,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="14">
         <f t="shared" si="3"/>
         <v>118</v>
@@ -4548,7 +4585,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="14">
         <f t="shared" si="3"/>
         <v>119</v>
@@ -4579,7 +4616,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="14">
         <f t="shared" si="3"/>
         <v>120</v>
@@ -4608,7 +4645,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="14">
         <f t="shared" si="3"/>
         <v>121</v>
@@ -4637,7 +4674,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="14">
         <f t="shared" si="3"/>
         <v>122</v>
@@ -4666,7 +4703,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="14">
         <f t="shared" si="3"/>
         <v>123</v>
@@ -4695,7 +4732,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="14">
         <f t="shared" si="3"/>
         <v>124</v>
@@ -4726,7 +4763,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="14">
         <f t="shared" si="3"/>
         <v>125</v>
@@ -4755,7 +4792,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="14">
         <f t="shared" si="3"/>
         <v>126</v>
@@ -4784,7 +4821,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="14">
         <f t="shared" si="3"/>
         <v>127</v>
@@ -4814,18 +4851,223 @@
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="14"/>
-      <c r="B129" s="5"/>
-      <c r="C129" s="16"/>
-      <c r="D129" s="16"/>
+      <c r="A129" s="14">
+        <f t="shared" si="3"/>
+        <v>128</v>
+      </c>
+      <c r="B129" s="5">
+        <v>44704</v>
+      </c>
+      <c r="C129" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D129" s="16">
+        <v>0.37152777777777773</v>
+      </c>
       <c r="E129" s="17">
-        <f>SUM(E2:E128)</f>
-        <v>3.2430555555555558</v>
-      </c>
-      <c r="F129" s="6"/>
-      <c r="G129" s="6"/>
-      <c r="H129" s="6"/>
-      <c r="I129" s="6"/>
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>3.819444444444442E-2</v>
+      </c>
+      <c r="F129" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G129" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="H129" s="7"/>
+      <c r="I129" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="14">
+        <f t="shared" si="3"/>
+        <v>129</v>
+      </c>
+      <c r="B130" s="5">
+        <v>44704</v>
+      </c>
+      <c r="C130" s="16">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="D130" s="16">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="E130" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>2.7777777777777846E-2</v>
+      </c>
+      <c r="F130" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G130" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="H130" s="7"/>
+      <c r="I130" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" s="14">
+        <f t="shared" si="3"/>
+        <v>130</v>
+      </c>
+      <c r="B131" s="5">
+        <v>44704</v>
+      </c>
+      <c r="C131" s="16">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D131" s="16">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="E131" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>2.4305555555555469E-2</v>
+      </c>
+      <c r="F131" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G131" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H131" s="7"/>
+      <c r="I131" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A132" s="14">
+        <f t="shared" si="3"/>
+        <v>131</v>
+      </c>
+      <c r="B132" s="5">
+        <v>44704</v>
+      </c>
+      <c r="C132" s="16">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="D132" s="16">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="E132" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G132" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H132" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="I132" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" s="14">
+        <f t="shared" si="3"/>
+        <v>132</v>
+      </c>
+      <c r="B133" s="5">
+        <v>44704</v>
+      </c>
+      <c r="C133" s="16">
+        <v>0.5625</v>
+      </c>
+      <c r="D133" s="16">
+        <v>0.59930555555555554</v>
+      </c>
+      <c r="E133" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>3.6805555555555536E-2</v>
+      </c>
+      <c r="F133" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G133" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H133" s="7"/>
+      <c r="I133" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="14">
+        <f t="shared" si="3"/>
+        <v>133</v>
+      </c>
+      <c r="B134" s="5">
+        <v>44704</v>
+      </c>
+      <c r="C134" s="16">
+        <v>0.59930555555555554</v>
+      </c>
+      <c r="D134" s="16">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E134" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>2.9166666666666674E-2</v>
+      </c>
+      <c r="F134" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G134" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="H134" s="7"/>
+      <c r="I134" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="14">
+        <f t="shared" si="3"/>
+        <v>134</v>
+      </c>
+      <c r="B135" s="5">
+        <v>44704</v>
+      </c>
+      <c r="C135" s="16">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="D135" s="16">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="E135" s="17">
+        <f>Tableau3[[#This Row],[Fin]]-Tableau3[[#This Row],[Début]]</f>
+        <v>5.902777777777779E-2</v>
+      </c>
+      <c r="F135" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G135" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="H135" s="7"/>
+      <c r="I135" s="12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="14"/>
+      <c r="B136" s="5"/>
+      <c r="C136" s="16"/>
+      <c r="D136" s="16"/>
+      <c r="E136" s="18">
+        <f>SUM(E2:E135)</f>
+        <v>3.4479166666666656</v>
+      </c>
+      <c r="F136" s="6"/>
+      <c r="G136" s="6"/>
+      <c r="H136" s="6"/>
+      <c r="I136" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -4857,7 +5099,7 @@
           <x14:formula1>
             <xm:f>'Types de Tâche'!$A$2:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F128</xm:sqref>
+          <xm:sqref>F2:F135</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>